<commit_message>
read new columns into json object
</commit_message>
<xml_diff>
--- a/__tests__/utils/ScenariosWith2023Q3RatesAndThresholds.xlsx
+++ b/__tests__/utils/ScenariosWith2023Q3RatesAndThresholds.xlsx
@@ -760,7 +760,7 @@
     <t>Birth Year and Month</t>
   </si>
   <si>
-    <t>Partner's Birth Year and Month</t>
+    <t>Partner Birth Year and Month</t>
   </si>
   <si>
     <t>Notes</t>
@@ -6005,7 +6005,7 @@
     <tableColumn name="Marital Status_x000a_(With or Without Partner, Widowed)" id="10"/>
     <tableColumn name="Inv Sep (Yes / No)" id="11"/>
     <tableColumn name="Partner's Age (Years and months)" id="12"/>
-    <tableColumn name="Partner's Birth Year and Month" id="13"/>
+    <tableColumn name="Partner Birth Year and Month" id="13"/>
     <tableColumn name="Partner's Net Worldwide Income" id="14"/>
     <tableColumn name="Combined Net Worldwide Income" id="15"/>
     <tableColumn name="Partner's Legal Status (Yes / No)" id="16"/>

</xml_diff>

<commit_message>
fixed tests that are passing
</commit_message>
<xml_diff>
--- a/__tests__/utils/ScenariosWith2023Q3RatesAndThresholds.xlsx
+++ b/__tests__/utils/ScenariosWith2023Q3RatesAndThresholds.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3375" uniqueCount="661">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3376" uniqueCount="661">
   <si>
     <t>Will be Eligible Test Scenarios</t>
   </si>
@@ -4927,7 +4927,7 @@
 ALWS = not eligible due to age
 Partner
 Eligible:
-OAS = 192.12 (with 10 years of residency at the earliest age of eligibility)
+OAS = 174.65 (with 10 years of residency at the earliest age of eligibility)
 GIS = Income too high
 ALW = not eligible due to age</t>
   </si>
@@ -18466,7 +18466,9 @@
       <c r="R196" s="101" t="s">
         <v>28</v>
       </c>
-      <c r="S196" s="103"/>
+      <c r="S196" s="103" t="s">
+        <v>55</v>
+      </c>
       <c r="T196" s="75" t="s">
         <v>660</v>
       </c>

</xml_diff>

<commit_message>
couple more tests, not all passing
</commit_message>
<xml_diff>
--- a/__tests__/utils/ScenariosWith2023Q3RatesAndThresholds.xlsx
+++ b/__tests__/utils/ScenariosWith2023Q3RatesAndThresholds.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3712" uniqueCount="723">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3698" uniqueCount="720">
   <si>
     <t>Will be Eligible Test Scenarios</t>
   </si>
@@ -5652,15 +5652,6 @@
   </si>
   <si>
     <t>CALC-197</t>
-  </si>
-  <si>
-    <t>$10,000.00</t>
-  </si>
-  <si>
-    <t>$35,000.00</t>
-  </si>
-  <si>
-    <t>$45,000.00</t>
   </si>
   <si>
     <t xml:space="preserve">User will be eligible for:
@@ -22041,14 +22032,14 @@
       <c r="E207" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F207" s="105" t="s">
-        <v>704</v>
-      </c>
-      <c r="G207" s="105" t="s">
-        <v>687</v>
-      </c>
-      <c r="H207" s="105" t="s">
-        <v>704</v>
+      <c r="F207" s="105">
+        <v>10000</v>
+      </c>
+      <c r="G207" s="105">
+        <v>0</v>
+      </c>
+      <c r="H207" s="105">
+        <v>10000</v>
       </c>
       <c r="I207" s="30" t="s">
         <v>23</v>
@@ -22071,17 +22062,17 @@
       <c r="O207" s="6" t="s">
         <v>701</v>
       </c>
-      <c r="P207" s="105" t="s">
-        <v>705</v>
-      </c>
-      <c r="Q207" s="105" t="s">
-        <v>687</v>
-      </c>
-      <c r="R207" s="105" t="s">
-        <v>705</v>
-      </c>
-      <c r="S207" s="107" t="s">
-        <v>706</v>
+      <c r="P207" s="105">
+        <v>35000</v>
+      </c>
+      <c r="Q207" s="105">
+        <v>0</v>
+      </c>
+      <c r="R207" s="105">
+        <v>35000</v>
+      </c>
+      <c r="S207" s="107">
+        <v>45000</v>
       </c>
       <c r="T207" s="30" t="s">
         <v>23</v>
@@ -22096,13 +22087,13 @@
         <v>22</v>
       </c>
       <c r="X207" s="13" t="s">
-        <v>707</v>
+        <v>704</v>
       </c>
       <c r="Y207" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="208" customHeight="1" ht="17.25">
       <c r="A208" s="103" t="s">
-        <v>708</v>
+        <v>705</v>
       </c>
       <c r="B208" s="104">
         <v>55</v>
@@ -22116,14 +22107,14 @@
       <c r="E208" s="30" t="s">
         <v>22</v>
       </c>
-      <c r="F208" s="105" t="s">
-        <v>687</v>
-      </c>
-      <c r="G208" s="105" t="s">
-        <v>687</v>
-      </c>
-      <c r="H208" s="105" t="s">
-        <v>687</v>
+      <c r="F208" s="105">
+        <v>0</v>
+      </c>
+      <c r="G208" s="105">
+        <v>0</v>
+      </c>
+      <c r="H208" s="105">
+        <v>0</v>
       </c>
       <c r="I208" s="30" t="s">
         <v>23</v>
@@ -22146,17 +22137,17 @@
       <c r="O208" s="6" t="s">
         <v>701</v>
       </c>
-      <c r="P208" s="105" t="s">
-        <v>687</v>
-      </c>
-      <c r="Q208" s="105" t="s">
-        <v>687</v>
-      </c>
-      <c r="R208" s="105" t="s">
-        <v>687</v>
-      </c>
-      <c r="S208" s="107" t="s">
-        <v>687</v>
+      <c r="P208" s="105">
+        <v>0</v>
+      </c>
+      <c r="Q208" s="105">
+        <v>0</v>
+      </c>
+      <c r="R208" s="105">
+        <v>0</v>
+      </c>
+      <c r="S208" s="107">
+        <v>0</v>
       </c>
       <c r="T208" s="30" t="s">
         <v>23</v>
@@ -22171,19 +22162,19 @@
         <v>22</v>
       </c>
       <c r="X208" s="13" t="s">
-        <v>709</v>
+        <v>706</v>
       </c>
       <c r="Y208" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="209" customHeight="1" ht="17.25">
       <c r="A209" s="103" t="s">
-        <v>710</v>
+        <v>707</v>
       </c>
       <c r="B209" s="108">
         <v>70</v>
       </c>
       <c r="C209" s="6" t="s">
-        <v>711</v>
+        <v>708</v>
       </c>
       <c r="D209" s="6" t="s">
         <v>47</v>
@@ -22246,19 +22237,19 @@
         <v>22</v>
       </c>
       <c r="X209" s="13" t="s">
-        <v>712</v>
+        <v>709</v>
       </c>
       <c r="Y209" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="210" customHeight="1" ht="17.25">
       <c r="A210" s="103" t="s">
-        <v>713</v>
+        <v>710</v>
       </c>
       <c r="B210" s="109">
         <v>68.75</v>
       </c>
       <c r="C210" s="6" t="s">
-        <v>714</v>
+        <v>711</v>
       </c>
       <c r="D210" s="6" t="s">
         <v>47</v>
@@ -22294,7 +22285,7 @@
         <v>59.25</v>
       </c>
       <c r="O210" s="6" t="s">
-        <v>715</v>
+        <v>712</v>
       </c>
       <c r="P210" s="16">
         <v>88000</v>
@@ -22321,19 +22312,19 @@
         <v>22</v>
       </c>
       <c r="X210" s="13" t="s">
-        <v>716</v>
+        <v>713</v>
       </c>
       <c r="Y210" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="211" customHeight="1" ht="17.25">
       <c r="A211" s="103" t="s">
-        <v>717</v>
+        <v>714</v>
       </c>
       <c r="B211" s="110">
         <v>59.92</v>
       </c>
       <c r="C211" s="6" t="s">
-        <v>718</v>
+        <v>715</v>
       </c>
       <c r="D211" s="111" t="s">
         <v>22</v>
@@ -22396,13 +22387,13 @@
         <v>55</v>
       </c>
       <c r="X211" s="53" t="s">
-        <v>719</v>
+        <v>716</v>
       </c>
       <c r="Y211" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="212" customHeight="1" ht="17.25">
       <c r="A212" s="103" t="s">
-        <v>720</v>
+        <v>717</v>
       </c>
       <c r="B212" s="110">
         <v>63.08</v>
@@ -22471,13 +22462,13 @@
         <v>22</v>
       </c>
       <c r="X212" s="13" t="s">
-        <v>721</v>
+        <v>718</v>
       </c>
       <c r="Y212" s="4"/>
     </row>
     <row x14ac:dyDescent="0.25" r="213" customHeight="1" ht="15">
       <c r="A213" s="6" t="s">
-        <v>722</v>
+        <v>719</v>
       </c>
       <c r="B213" s="29">
         <v>75.17</v>

</xml_diff>